<commit_message>
#14 - Testes finais
</commit_message>
<xml_diff>
--- a/dist/resultados_modelos.xlsx
+++ b/dist/resultados_modelos.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>status</t>
   </si>
   <si>
+    <t>var</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -31,9 +34,24 @@
     <t>time</t>
   </si>
   <si>
+    <t>scores</t>
+  </si>
+  <si>
+    <t>caminho</t>
+  </si>
+  <si>
     <t>ok</t>
   </si>
   <si>
+    <t>appetency</t>
+  </si>
+  <si>
+    <t>churn</t>
+  </si>
+  <si>
+    <t>upselling</t>
+  </si>
+  <si>
     <t>GradientBoostingClassifier</t>
   </si>
   <si>
@@ -44,6 +62,134 @@
   </si>
   <si>
     <t>KNeighborsClassifier</t>
+  </si>
+  <si>
+    <t>LinearSVC</t>
+  </si>
+  <si>
+    <t>SGDClassifier</t>
+  </si>
+  <si>
+    <t>[0.98019802 0.98019802 0.97029703 0.96039604 0.97       0.98
+ 0.98989899 0.98989899 0.95959596 0.98989899]</t>
+  </si>
+  <si>
+    <t>[0.98019802 0.98019802 0.98019802 0.98019802 0.99       0.99
+ 0.98989899 0.98989899 0.98989899 0.98989899]</t>
+  </si>
+  <si>
+    <t>[0.97029703 0.97029703 0.96039604 0.95049505 0.96       0.95
+ 0.96969697 0.98989899 0.94949495 0.98989899]</t>
+  </si>
+  <si>
+    <t>[0.66336634 0.96039604 0.87128713 0.96039604 0.98       0.94
+ 0.92929293 0.60606061 0.84848485 0.97979798]</t>
+  </si>
+  <si>
+    <t>[0.98019802 0.95049505 0.98019802 0.96039604 0.89       0.99
+ 0.97979798 0.94949495 0.98989899 0.98989899]</t>
+  </si>
+  <si>
+    <t>[0.94059406 0.94       0.92       0.94       0.92       0.93
+ 0.93       0.94       0.94       0.93939394]</t>
+  </si>
+  <si>
+    <t>[0.94059406 0.94       0.94       0.94       0.94       0.94
+ 0.93       0.94       0.93       0.94949495]</t>
+  </si>
+  <si>
+    <t>[0.82178218 0.89       0.84       0.87       0.83       0.9
+ 0.88       0.89       0.88       0.88888889]</t>
+  </si>
+  <si>
+    <t>[0.93069307 0.94       0.93       0.94       0.95       0.94
+ 0.93       0.94       0.94       0.94949495]</t>
+  </si>
+  <si>
+    <t>[0.71287129 0.83       0.55       0.6        0.89       0.91
+ 0.93       0.85       0.77       0.94949495]</t>
+  </si>
+  <si>
+    <t>[0.89108911 0.92       0.94       0.92       0.84       0.79
+ 0.94       0.35       0.94       0.85858586]</t>
+  </si>
+  <si>
+    <t>[0.9009901  0.93069307 0.91       0.97       0.94       0.92
+ 0.94       0.94       0.90909091 0.95959596]</t>
+  </si>
+  <si>
+    <t>[0.9009901  0.9009901  0.91       0.93       0.91       0.91
+ 0.91       0.91       0.92929293 0.90909091]</t>
+  </si>
+  <si>
+    <t>[0.85148515 0.91089109 0.86       0.93       0.85       0.86
+ 0.85       0.87       0.86868687 0.83838384]</t>
+  </si>
+  <si>
+    <t>[0.9009901  0.9009901  0.91       0.88       0.87       0.91
+ 0.9        0.91       0.8989899  0.91919192]</t>
+  </si>
+  <si>
+    <t>[0.77227723 0.77227723 0.87       0.64       0.86       0.7
+ 0.84       0.59       0.78787879 0.90909091]</t>
+  </si>
+  <si>
+    <t>[0.89108911 0.88118812 0.79       0.85       0.91       0.87
+ 0.91       0.85       0.87878788 0.90909091]</t>
+  </si>
+  <si>
+    <t>../../models/appetency_GradientBoostingClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/appetency_RandomForestClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/appetency_DecisionTreeClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/appetency_KNeighborsClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/appetency_LinearSVC.model</t>
+  </si>
+  <si>
+    <t>../../models/appetency_SGDClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_GradientBoostingClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_RandomForestClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_DecisionTreeClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_KNeighborsClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_LinearSVC.model</t>
+  </si>
+  <si>
+    <t>../../models/churn_SGDClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_GradientBoostingClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_RandomForestClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_DecisionTreeClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_KNeighborsClassifier.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_LinearSVC.model</t>
+  </si>
+  <si>
+    <t>../../models/upselling_SGDClassifier.model</t>
   </si>
 </sst>
 </file>
@@ -401,13 +547,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,209 +569,482 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>0.9814000000000001</v>
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>0.0004098780306383821</v>
+        <v>0.977038203820382</v>
       </c>
       <c r="E2">
-        <v>154.886307477951</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.01095953384616845</v>
+      </c>
+      <c r="F2">
+        <v>2.743458032608032</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>0.9821199999999999</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>0.0001326649916142014</v>
+        <v>0.986038803880388</v>
       </c>
       <c r="E3">
-        <v>19.45039939880371</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.004769122858463881</v>
+      </c>
+      <c r="F3">
+        <v>0.176161527633667</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>0.96122</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.001778651174345306</v>
+        <v>0.9660475047504751</v>
       </c>
       <c r="E4">
-        <v>32.80617165565491</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.01424472511842958</v>
+      </c>
+      <c r="F4">
+        <v>0.1846988201141357</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>0.9821200000000001</v>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>9.797958971131634e-05</v>
+        <v>0.986038803880388</v>
       </c>
       <c r="E5">
-        <v>20.09524869918823</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.004769122858463881</v>
+      </c>
+      <c r="F5">
+        <v>0.06261348724365234</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>0.926360030819201</v>
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>0.0006824782128912647</v>
+        <v>0.8739081908190819</v>
       </c>
       <c r="E6">
-        <v>164.8802347183228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.1271170441693648</v>
+      </c>
+      <c r="F6">
+        <v>0.7755062580108643</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>0.9257600628032024</v>
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>0.0009147782333925092</v>
+        <v>0.966037803780378</v>
       </c>
       <c r="E7">
-        <v>23.8265221118927</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.02938041095419672</v>
+      </c>
+      <c r="F7">
+        <v>0.03612422943115234</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>0.8619201977856079</v>
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>0.00526431441001887</v>
+        <v>0.9339987998799879</v>
       </c>
       <c r="E8">
-        <v>39.56057143211365</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.008003600360035968</v>
+      </c>
+      <c r="F8">
+        <v>2.884362936019897</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0.9232199547783981</v>
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>0.0007337440982491631</v>
+        <v>0.939008900890089</v>
       </c>
       <c r="E9">
-        <v>19.58282876014709</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>0.005297963741219471</v>
+      </c>
+      <c r="F9">
+        <v>0.3246090412139893</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>0.9506999711895988</v>
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.001819201858717591</v>
+        <v>0.869067106710671</v>
       </c>
       <c r="E10">
-        <v>154.8306312561035</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>0.02659519799133285</v>
+      </c>
+      <c r="F10">
+        <v>0.438051700592041</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>0.9456800511224021</v>
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
       </c>
       <c r="D11">
-        <v>0.002091073835534662</v>
+        <v>0.9390188018801879</v>
       </c>
       <c r="E11">
-        <v>21.47616720199585</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>0.006834804513181102</v>
+      </c>
+      <c r="F11">
+        <v>0.06551837921142578</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>0.9044998984823959</v>
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>0.00382462056005061</v>
+        <v>0.7992366236623661</v>
       </c>
       <c r="E12">
-        <v>32.62160277366638</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>0.1318462457170382</v>
+      </c>
+      <c r="F12">
+        <v>1.022980690002441</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>0.9215600987480039</v>
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
       </c>
       <c r="D13">
-        <v>0.001525417175957127</v>
+        <v>0.8389674967496749</v>
       </c>
       <c r="E13">
-        <v>19.70243310928345</v>
+        <v>0.1698072055476631</v>
+      </c>
+      <c r="F13">
+        <v>0.03125572204589844</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0.93203700370037</v>
+      </c>
+      <c r="E14">
+        <v>0.02124540366012526</v>
+      </c>
+      <c r="F14">
+        <v>2.929417133331299</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>0.912036403640364</v>
+      </c>
+      <c r="E15">
+        <v>0.009454791382261463</v>
+      </c>
+      <c r="F15">
+        <v>0.2999813556671143</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>0.8689446944694469</v>
+      </c>
+      <c r="E16">
+        <v>0.02757725545732684</v>
+      </c>
+      <c r="F16">
+        <v>0.3694536685943604</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0.9000162016201619</v>
+      </c>
+      <c r="E17">
+        <v>0.0140403277507814</v>
+      </c>
+      <c r="F17">
+        <v>0.06900477409362793</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>0.7741524152415242</v>
+      </c>
+      <c r="E18">
+        <v>0.09833812996827453</v>
+      </c>
+      <c r="F18">
+        <v>1.308091878890991</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>0.874015601560156</v>
+      </c>
+      <c r="E19">
+        <v>0.03523350670235521</v>
+      </c>
+      <c r="F19">
+        <v>0.04311466217041016</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes #14 , Fixes #13
</commit_message>
<xml_diff>
--- a/dist/resultados_modelos.xlsx
+++ b/dist/resultados_modelos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>status</t>
   </si>
@@ -70,72 +70,70 @@
     <t>SGDClassifier</t>
   </si>
   <si>
-    <t>[0.98019802 0.98019802 0.97029703 0.96039604 0.97       0.98
- 0.98989899 0.98989899 0.95959596 0.98989899]</t>
-  </si>
-  <si>
-    <t>[0.98019802 0.98019802 0.98019802 0.98019802 0.99       0.99
- 0.98989899 0.98989899 0.98989899 0.98989899]</t>
-  </si>
-  <si>
-    <t>[0.97029703 0.97029703 0.96039604 0.95049505 0.96       0.95
- 0.96969697 0.98989899 0.94949495 0.98989899]</t>
-  </si>
-  <si>
-    <t>[0.66336634 0.96039604 0.87128713 0.96039604 0.98       0.94
- 0.92929293 0.60606061 0.84848485 0.97979798]</t>
-  </si>
-  <si>
-    <t>[0.98019802 0.95049505 0.98019802 0.96039604 0.89       0.99
- 0.97979798 0.94949495 0.98989899 0.98989899]</t>
-  </si>
-  <si>
-    <t>[0.94059406 0.94       0.92       0.94       0.92       0.93
- 0.93       0.94       0.94       0.93939394]</t>
-  </si>
-  <si>
-    <t>[0.94059406 0.94       0.94       0.94       0.94       0.94
- 0.93       0.94       0.93       0.94949495]</t>
-  </si>
-  <si>
-    <t>[0.82178218 0.89       0.84       0.87       0.83       0.9
- 0.88       0.89       0.88       0.88888889]</t>
-  </si>
-  <si>
-    <t>[0.93069307 0.94       0.93       0.94       0.95       0.94
- 0.93       0.94       0.94       0.94949495]</t>
-  </si>
-  <si>
-    <t>[0.71287129 0.83       0.55       0.6        0.89       0.91
- 0.93       0.85       0.77       0.94949495]</t>
-  </si>
-  <si>
-    <t>[0.89108911 0.92       0.94       0.92       0.84       0.79
- 0.94       0.35       0.94       0.85858586]</t>
-  </si>
-  <si>
-    <t>[0.9009901  0.93069307 0.91       0.97       0.94       0.92
- 0.94       0.94       0.90909091 0.95959596]</t>
-  </si>
-  <si>
-    <t>[0.9009901  0.9009901  0.91       0.93       0.91       0.91
- 0.91       0.91       0.92929293 0.90909091]</t>
-  </si>
-  <si>
-    <t>[0.85148515 0.91089109 0.86       0.93       0.85       0.86
- 0.85       0.87       0.86868687 0.83838384]</t>
-  </si>
-  <si>
-    <t>[0.9009901  0.9009901  0.91       0.88       0.87       0.91
- 0.9        0.91       0.8989899  0.91919192]</t>
-  </si>
-  <si>
-    <t>[0.77227723 0.77227723 0.87       0.64       0.86       0.7
- 0.84       0.59       0.78787879 0.90909091]</t>
-  </si>
-  <si>
-    <t>[0.89108911 0.88118812 0.79       0.85       0.91       0.87
- 0.91       0.85       0.87878788 0.90909091]</t>
+    <t>[0.9816 0.9806 0.9812 0.9818 0.9812 0.9816 0.9812 0.982  0.9812 0.982 ]</t>
+  </si>
+  <si>
+    <t>[0.9822 0.982  0.9822 0.9822 0.982  0.9822 0.9822 0.9822 0.9822 0.982 ]</t>
+  </si>
+  <si>
+    <t>[0.9594 0.9622 0.9618 0.9616 0.9632 0.9618 0.9582 0.9624 0.9594 0.9608]</t>
+  </si>
+  <si>
+    <t>[0.9822 0.982  0.982  0.982  0.9822 0.9822 0.9822 0.982  0.9822 0.9822]</t>
+  </si>
+  <si>
+    <t>[0.9346 0.7938 0.9522 0.3134 0.9514 0.4898 0.7978 0.5832 0.8014 0.9456]</t>
+  </si>
+  <si>
+    <t>[0.974  0.9762 0.9766 0.975  0.9082 0.9758 0.9776 0.9616 0.9754 0.972 ]</t>
+  </si>
+  <si>
+    <t>[0.92661468 0.92521496 0.9258     0.9266     0.926      0.9268
+ 0.9274     0.9254     0.92738548 0.92578516]</t>
+  </si>
+  <si>
+    <t>[0.92521496 0.92481504 0.9244     0.9266     0.9254     0.9264
+ 0.9252     0.9264     0.92558512 0.92558512]</t>
+  </si>
+  <si>
+    <t>[0.86262747 0.85222955 0.8596     0.8654     0.8526     0.8684
+ 0.8608     0.8664     0.86057211 0.86637327]</t>
+  </si>
+  <si>
+    <t>[0.92381524 0.92461508 0.9228     0.9228     0.9222     0.9238
+ 0.9224     0.9236     0.92258452 0.92358472]</t>
+  </si>
+  <si>
+    <t>[0.52509498 0.45490902 0.9134     0.351      0.3746     0.8064
+ 0.4496     0.5014     0.68993799 0.52310462]</t>
+  </si>
+  <si>
+    <t>[0.84283143 0.910018   0.9158     0.9188     0.2192     0.913
+ 0.9156     0.9136     0.21464293 0.91358272]</t>
+  </si>
+  <si>
+    <t>[0.94981004 0.94961008 0.952      0.9506     0.9498     0.9526
+ 0.9518     0.9528     0.95179036 0.94638928]</t>
+  </si>
+  <si>
+    <t>[0.945011   0.94621076 0.9456     0.947      0.9442     0.9488
+ 0.9458     0.9492     0.944989   0.94318864]</t>
+  </si>
+  <si>
+    <t>[0.90421916 0.90321936 0.9034     0.9016     0.9024     0.9074
+ 0.907      0.9116     0.90538108 0.90558112]</t>
+  </si>
+  <si>
+    <t>[0.92041592 0.92061588 0.9248     0.92       0.9222     0.9202
+ 0.9206     0.9208     0.92258452 0.92338468]</t>
+  </si>
+  <si>
+    <t>[0.75284943 0.48510298 0.3636     0.6482     0.6484     0.7396
+ 0.7634     0.5386     0.27925585 0.4554911 ]</t>
+  </si>
+  <si>
+    <t>[0.90281944 0.91661668 0.9176     0.9156     0.9164     0.2348
+ 0.913      0.9098     0.85217043 0.91738348]</t>
   </si>
   <si>
     <t>../../models/appetency_GradientBoostingClassifier.model</t>
@@ -590,19 +588,19 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>0.977038203820382</v>
+        <v>0.9814399999999999</v>
       </c>
       <c r="E2">
-        <v>0.01095953384616845</v>
+        <v>0.0004176122603564239</v>
       </c>
       <c r="F2">
-        <v>2.743458032608032</v>
+        <v>154.2975769042969</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -616,19 +614,19 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>0.986038803880388</v>
+        <v>0.9821399999999999</v>
       </c>
       <c r="E3">
-        <v>0.004769122858463881</v>
+        <v>9.165151389910671e-05</v>
       </c>
       <c r="F3">
-        <v>0.176161527633667</v>
+        <v>18.78320002555847</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -642,19 +640,19 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>0.9660475047504751</v>
+        <v>0.9610800000000002</v>
       </c>
       <c r="E4">
-        <v>0.01424472511842958</v>
+        <v>0.001510496607079919</v>
       </c>
       <c r="F4">
-        <v>0.1846988201141357</v>
+        <v>31.44332933425903</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -668,19 +666,19 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>0.986038803880388</v>
+        <v>0.9821200000000001</v>
       </c>
       <c r="E5">
-        <v>0.004769122858463881</v>
+        <v>9.797958971131634e-05</v>
       </c>
       <c r="F5">
-        <v>0.06261348724365234</v>
+        <v>19.77473402023315</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -694,19 +692,19 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>0.8739081908190819</v>
+        <v>0.75632</v>
       </c>
       <c r="E6">
-        <v>0.1271170441693648</v>
+        <v>0.2112758803081885</v>
       </c>
       <c r="F6">
-        <v>0.7755062580108643</v>
+        <v>152.2808775901794</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -720,19 +718,19 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>0.966037803780378</v>
+        <v>0.96724</v>
       </c>
       <c r="E7">
-        <v>0.02938041095419672</v>
+        <v>0.02015237951210725</v>
       </c>
       <c r="F7">
-        <v>0.03612422943115234</v>
+        <v>1.035181045532227</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -746,19 +744,19 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>0.9339987998799879</v>
+        <v>0.926300026820001</v>
       </c>
       <c r="E8">
-        <v>0.008003600360035968</v>
+        <v>0.0007361836556161717</v>
       </c>
       <c r="F8">
-        <v>2.884362936019897</v>
+        <v>161.7057368755341</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -772,19 +770,19 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>0.939008900890089</v>
+        <v>0.9255600228048009</v>
       </c>
       <c r="E9">
-        <v>0.005297963741219471</v>
+        <v>0.0006832924902877616</v>
       </c>
       <c r="F9">
-        <v>0.3246090412139893</v>
+        <v>25.04467844963074</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -798,19 +796,19 @@
         <v>14</v>
       </c>
       <c r="D10">
-        <v>0.869067106710671</v>
+        <v>0.8615002417672096</v>
       </c>
       <c r="E10">
-        <v>0.02659519799133285</v>
+        <v>0.005310010763333176</v>
       </c>
       <c r="F10">
-        <v>0.438051700592041</v>
+        <v>38.10170459747314</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -824,19 +822,19 @@
         <v>15</v>
       </c>
       <c r="D11">
-        <v>0.9390188018801879</v>
+        <v>0.9232199547783981</v>
       </c>
       <c r="E11">
-        <v>0.006834804513181102</v>
+        <v>0.0007337440982491631</v>
       </c>
       <c r="F11">
-        <v>0.06551837921142578</v>
+        <v>19.07599210739136</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -850,19 +848,19 @@
         <v>16</v>
       </c>
       <c r="D12">
-        <v>0.7992366236623661</v>
+        <v>0.5589446607721865</v>
       </c>
       <c r="E12">
-        <v>0.1318462457170382</v>
+        <v>0.17600491101579</v>
       </c>
       <c r="F12">
-        <v>1.022980690002441</v>
+        <v>154.9204533100128</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -876,19 +874,19 @@
         <v>17</v>
       </c>
       <c r="D13">
-        <v>0.8389674967496749</v>
+        <v>0.7677075075243003</v>
       </c>
       <c r="E13">
-        <v>0.1698072055476631</v>
+        <v>0.2762143035932596</v>
       </c>
       <c r="F13">
-        <v>0.03125572204589844</v>
+        <v>1.008742570877075</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -902,19 +900,19 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>0.93203700370037</v>
+        <v>0.950719975190399</v>
       </c>
       <c r="E14">
-        <v>0.02124540366012526</v>
+        <v>0.00182995022947457</v>
       </c>
       <c r="F14">
-        <v>2.929417133331299</v>
+        <v>147.6034967899323</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -928,19 +926,19 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>0.912036403640364</v>
+        <v>0.9459999391175975</v>
       </c>
       <c r="E15">
-        <v>0.009454791382261463</v>
+        <v>0.001801899760270206</v>
       </c>
       <c r="F15">
-        <v>0.2999813556671143</v>
+        <v>20.7317168712616</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -954,19 +952,19 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>0.8689446944694469</v>
+        <v>0.9051800704736028</v>
       </c>
       <c r="E16">
-        <v>0.02757725545732684</v>
+        <v>0.002795336671619653</v>
       </c>
       <c r="F16">
-        <v>0.3694536685943604</v>
+        <v>33.20013284683228</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -980,19 +978,19 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>0.9000162016201619</v>
+        <v>0.9215600987480039</v>
       </c>
       <c r="E17">
-        <v>0.0140403277507814</v>
+        <v>0.001525417175957127</v>
       </c>
       <c r="F17">
-        <v>0.06900477409362793</v>
+        <v>19.30067324638367</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1006,19 +1004,19 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>0.7741524152415242</v>
+        <v>0.5674499358907974</v>
       </c>
       <c r="E18">
-        <v>0.09833812996827453</v>
+        <v>0.1613187151557877</v>
       </c>
       <c r="F18">
-        <v>1.308091878890991</v>
+        <v>152.740654706955</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1032,19 +1030,19 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>0.874015601560156</v>
+        <v>0.8396190023559601</v>
       </c>
       <c r="E19">
-        <v>0.03523350670235521</v>
+        <v>0.2024829442288751</v>
       </c>
       <c r="F19">
-        <v>0.04311466217041016</v>
+        <v>0.995389461517334</v>
       </c>
       <c r="G19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>